<commit_message>
Enhance recommendation prompt with Expert Local Guide persona and refine search top_k
</commit_message>
<xml_diff>
--- a/Cairo_Giza_POI_Database_v3.xlsx
+++ b/Cairo_Giza_POI_Database_v3.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abraam Refaat\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abraam Refaat\Downloads\travel-recommendation-api---main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DE98014-FD73-4B98-970C-961EA64FA0EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9BC6FC9-095E-429A-8682-BC988D6AA562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,14 +17,14 @@
     <sheet name="Summary" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Cairo &amp; Giza POIs'!$A$1:$H$212</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Cairo &amp; Giza POIs'!$A$1:$H$210</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1498" uniqueCount="488">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1484" uniqueCount="484">
   <si>
     <t>Name</t>
   </si>
@@ -794,12 +794,6 @@
     <t>29.898, 31.205</t>
   </si>
   <si>
-    <t>Pyramid of Pepi I (South Saqqara)</t>
-  </si>
-  <si>
-    <t>29.857, 31.222</t>
-  </si>
-  <si>
     <t>Pyramid of Sahure</t>
   </si>
   <si>
@@ -948,12 +942,6 @@
   </si>
   <si>
     <t>29.872, 31.214</t>
-  </si>
-  <si>
-    <t>Wadi El Natrun Day Trip (from Cairo)</t>
-  </si>
-  <si>
-    <t>30.35, 30.32</t>
   </si>
   <si>
     <t>Al Horreya Garden</t>
@@ -2022,11 +2010,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H212"/>
+  <dimension ref="A1:H210"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A60" sqref="A60"/>
+      <pane ySplit="1" topLeftCell="A197" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A108" sqref="A108:XFD108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4836,7 +4824,7 @@
         <v>218</v>
       </c>
       <c r="E108" s="6" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F108" s="7">
         <v>0</v>
@@ -4862,7 +4850,7 @@
         <v>218</v>
       </c>
       <c r="E109" s="6" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="F109" s="7">
         <v>0</v>
@@ -4888,13 +4876,13 @@
         <v>218</v>
       </c>
       <c r="E110" s="6" t="s">
-        <v>84</v>
+        <v>17</v>
       </c>
       <c r="F110" s="7">
         <v>0</v>
       </c>
       <c r="G110" s="6" t="s">
-        <v>219</v>
+        <v>75</v>
       </c>
       <c r="H110" s="6" t="s">
         <v>31</v>
@@ -4914,13 +4902,13 @@
         <v>218</v>
       </c>
       <c r="E111" s="6" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="F111" s="7">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="G111" s="6" t="s">
-        <v>75</v>
+        <v>219</v>
       </c>
       <c r="H111" s="6" t="s">
         <v>31</v>
@@ -4940,10 +4928,10 @@
         <v>218</v>
       </c>
       <c r="E112" s="6" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="F112" s="7">
-        <v>200</v>
+        <v>450</v>
       </c>
       <c r="G112" s="6" t="s">
         <v>219</v>
@@ -4966,10 +4954,10 @@
         <v>218</v>
       </c>
       <c r="E113" s="6" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="F113" s="7">
-        <v>450</v>
+        <v>0</v>
       </c>
       <c r="G113" s="6" t="s">
         <v>219</v>
@@ -4983,7 +4971,7 @@
         <v>268</v>
       </c>
       <c r="B114" s="6" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C114" s="6" t="s">
         <v>68</v>
@@ -4992,7 +4980,7 @@
         <v>218</v>
       </c>
       <c r="E114" s="6" t="s">
-        <v>17</v>
+        <v>81</v>
       </c>
       <c r="F114" s="7">
         <v>0</v>
@@ -5006,10 +4994,10 @@
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A115" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="B115" s="6" t="s">
         <v>270</v>
-      </c>
-      <c r="B115" s="6" t="s">
-        <v>269</v>
       </c>
       <c r="C115" s="6" t="s">
         <v>68</v>
@@ -5018,13 +5006,13 @@
         <v>218</v>
       </c>
       <c r="E115" s="6" t="s">
-        <v>81</v>
+        <v>17</v>
       </c>
       <c r="F115" s="7">
         <v>0</v>
       </c>
       <c r="G115" s="6" t="s">
-        <v>219</v>
+        <v>75</v>
       </c>
       <c r="H115" s="6" t="s">
         <v>31</v>
@@ -5035,7 +5023,7 @@
         <v>271</v>
       </c>
       <c r="B116" s="6" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="C116" s="6" t="s">
         <v>68</v>
@@ -5050,7 +5038,7 @@
         <v>0</v>
       </c>
       <c r="G116" s="6" t="s">
-        <v>75</v>
+        <v>219</v>
       </c>
       <c r="H116" s="6" t="s">
         <v>31</v>
@@ -5058,10 +5046,10 @@
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A117" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="B117" s="6" t="s">
         <v>273</v>
-      </c>
-      <c r="B117" s="6" t="s">
-        <v>267</v>
       </c>
       <c r="C117" s="6" t="s">
         <v>68</v>
@@ -5096,7 +5084,7 @@
         <v>218</v>
       </c>
       <c r="E118" s="6" t="s">
-        <v>17</v>
+        <v>84</v>
       </c>
       <c r="F118" s="7">
         <v>0</v>
@@ -5122,7 +5110,7 @@
         <v>218</v>
       </c>
       <c r="E119" s="6" t="s">
-        <v>84</v>
+        <v>17</v>
       </c>
       <c r="F119" s="7">
         <v>0</v>
@@ -5148,13 +5136,13 @@
         <v>218</v>
       </c>
       <c r="E120" s="6" t="s">
-        <v>17</v>
+        <v>81</v>
       </c>
       <c r="F120" s="7">
         <v>0</v>
       </c>
       <c r="G120" s="6" t="s">
-        <v>219</v>
+        <v>75</v>
       </c>
       <c r="H120" s="6" t="s">
         <v>31</v>
@@ -5174,13 +5162,13 @@
         <v>218</v>
       </c>
       <c r="E121" s="6" t="s">
-        <v>81</v>
+        <v>17</v>
       </c>
       <c r="F121" s="7">
         <v>0</v>
       </c>
       <c r="G121" s="6" t="s">
-        <v>75</v>
+        <v>219</v>
       </c>
       <c r="H121" s="6" t="s">
         <v>31</v>
@@ -5197,68 +5185,68 @@
         <v>68</v>
       </c>
       <c r="D122" s="6" t="s">
-        <v>218</v>
+        <v>284</v>
       </c>
       <c r="E122" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="F122" s="7">
+        <v>0</v>
+      </c>
+      <c r="G122" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="H122" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A123" s="8" t="s">
+        <v>285</v>
+      </c>
+      <c r="B123" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="C123" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="D123" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="E123" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="F122" s="7">
-        <v>0</v>
-      </c>
-      <c r="G122" s="6" t="s">
-        <v>219</v>
-      </c>
-      <c r="H122" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A123" s="5" t="s">
-        <v>284</v>
-      </c>
-      <c r="B123" s="6" t="s">
-        <v>285</v>
-      </c>
-      <c r="C123" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="D123" s="6" t="s">
-        <v>286</v>
-      </c>
-      <c r="E123" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="F123" s="7">
-        <v>0</v>
-      </c>
-      <c r="G123" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="H123" s="6" t="s">
+      <c r="F123" s="10">
+        <v>10</v>
+      </c>
+      <c r="G123" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="H123" s="9" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A124" s="8" t="s">
+        <v>289</v>
+      </c>
+      <c r="B124" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="C124" s="9" t="s">
         <v>287</v>
       </c>
-      <c r="B124" s="9" t="s">
+      <c r="D124" s="9" t="s">
         <v>288</v>
       </c>
-      <c r="C124" s="9" t="s">
-        <v>289</v>
-      </c>
-      <c r="D124" s="9" t="s">
-        <v>290</v>
-      </c>
       <c r="E124" s="9" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="F124" s="10">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G124" s="9" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="H124" s="9" t="s">
         <v>31</v>
@@ -5272,13 +5260,13 @@
         <v>292</v>
       </c>
       <c r="C125" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D125" s="9" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="E125" s="9" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="F125" s="10">
         <v>5</v>
@@ -5292,25 +5280,25 @@
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A126" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="B126" s="9" t="s">
+        <v>295</v>
+      </c>
+      <c r="C126" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="D126" s="9" t="s">
         <v>293</v>
       </c>
-      <c r="B126" s="9" t="s">
-        <v>294</v>
-      </c>
-      <c r="C126" s="9" t="s">
-        <v>289</v>
-      </c>
-      <c r="D126" s="9" t="s">
-        <v>295</v>
-      </c>
       <c r="E126" s="9" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="F126" s="10">
-        <v>5</v>
+        <v>200</v>
       </c>
       <c r="G126" s="9" t="s">
-        <v>75</v>
+        <v>219</v>
       </c>
       <c r="H126" s="9" t="s">
         <v>31</v>
@@ -5324,19 +5312,19 @@
         <v>297</v>
       </c>
       <c r="C127" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D127" s="9" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E127" s="9" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F127" s="10">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="G127" s="9" t="s">
-        <v>219</v>
+        <v>106</v>
       </c>
       <c r="H127" s="9" t="s">
         <v>31</v>
@@ -5350,19 +5338,19 @@
         <v>299</v>
       </c>
       <c r="C128" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D128" s="9" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E128" s="9" t="s">
-        <v>17</v>
+        <v>84</v>
       </c>
       <c r="F128" s="10">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="G128" s="9" t="s">
-        <v>106</v>
+        <v>20</v>
       </c>
       <c r="H128" s="9" t="s">
         <v>31</v>
@@ -5376,19 +5364,19 @@
         <v>301</v>
       </c>
       <c r="C129" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D129" s="9" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E129" s="9" t="s">
-        <v>84</v>
+        <v>25</v>
       </c>
       <c r="F129" s="10">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="G129" s="9" t="s">
-        <v>20</v>
+        <v>75</v>
       </c>
       <c r="H129" s="9" t="s">
         <v>31</v>
@@ -5402,10 +5390,10 @@
         <v>303</v>
       </c>
       <c r="C130" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D130" s="9" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E130" s="9" t="s">
         <v>25</v>
@@ -5414,7 +5402,7 @@
         <v>0</v>
       </c>
       <c r="G130" s="9" t="s">
-        <v>75</v>
+        <v>106</v>
       </c>
       <c r="H130" s="9" t="s">
         <v>31</v>
@@ -5428,19 +5416,19 @@
         <v>305</v>
       </c>
       <c r="C131" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D131" s="9" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E131" s="9" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F131" s="10">
         <v>0</v>
       </c>
       <c r="G131" s="9" t="s">
-        <v>106</v>
+        <v>219</v>
       </c>
       <c r="H131" s="9" t="s">
         <v>31</v>
@@ -5451,13 +5439,13 @@
         <v>306</v>
       </c>
       <c r="B132" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="C132" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="D132" s="9" t="s">
         <v>307</v>
-      </c>
-      <c r="C132" s="9" t="s">
-        <v>289</v>
-      </c>
-      <c r="D132" s="9" t="s">
-        <v>295</v>
       </c>
       <c r="E132" s="9" t="s">
         <v>17</v>
@@ -5466,7 +5454,7 @@
         <v>0</v>
       </c>
       <c r="G132" s="9" t="s">
-        <v>219</v>
+        <v>308</v>
       </c>
       <c r="H132" s="9" t="s">
         <v>31</v>
@@ -5474,25 +5462,25 @@
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A133" s="8" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="B133" s="9" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C133" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D133" s="9" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="E133" s="9" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="F133" s="10">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="G133" s="9" t="s">
-        <v>106</v>
+        <v>311</v>
       </c>
       <c r="H133" s="9" t="s">
         <v>31</v>
@@ -5500,25 +5488,25 @@
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A134" s="8" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="B134" s="9" t="s">
-        <v>92</v>
+        <v>313</v>
       </c>
       <c r="C134" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D134" s="9" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="E134" s="9" t="s">
         <v>17</v>
       </c>
       <c r="F134" s="10">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G134" s="9" t="s">
-        <v>312</v>
+        <v>20</v>
       </c>
       <c r="H134" s="9" t="s">
         <v>31</v>
@@ -5526,25 +5514,25 @@
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A135" s="8" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B135" s="9" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C135" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D135" s="9" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="E135" s="9" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="F135" s="10">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="G135" s="9" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="H135" s="9" t="s">
         <v>31</v>
@@ -5552,25 +5540,25 @@
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A136" s="8" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="B136" s="9" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C136" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D136" s="9" t="s">
+        <v>307</v>
+      </c>
+      <c r="E136" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F136" s="10">
+        <v>30</v>
+      </c>
+      <c r="G136" s="9" t="s">
         <v>311</v>
-      </c>
-      <c r="E136" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F136" s="10">
-        <v>20</v>
-      </c>
-      <c r="G136" s="9" t="s">
-        <v>20</v>
       </c>
       <c r="H136" s="9" t="s">
         <v>31</v>
@@ -5578,16 +5566,16 @@
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A137" s="8" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B137" s="9" t="s">
-        <v>319</v>
+        <v>9</v>
       </c>
       <c r="C137" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D137" s="9" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="E137" s="9" t="s">
         <v>12</v>
@@ -5596,7 +5584,7 @@
         <v>0</v>
       </c>
       <c r="G137" s="9" t="s">
-        <v>320</v>
+        <v>311</v>
       </c>
       <c r="H137" s="9" t="s">
         <v>31</v>
@@ -5604,25 +5592,25 @@
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A138" s="8" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B138" s="9" t="s">
-        <v>322</v>
+        <v>190</v>
       </c>
       <c r="C138" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D138" s="9" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="E138" s="9" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="F138" s="10">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="G138" s="9" t="s">
-        <v>315</v>
+        <v>69</v>
       </c>
       <c r="H138" s="9" t="s">
         <v>31</v>
@@ -5630,25 +5618,25 @@
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A139" s="8" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B139" s="9" t="s">
-        <v>9</v>
+        <v>322</v>
       </c>
       <c r="C139" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D139" s="9" t="s">
+        <v>307</v>
+      </c>
+      <c r="E139" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F139" s="10">
+        <v>20</v>
+      </c>
+      <c r="G139" s="9" t="s">
         <v>311</v>
-      </c>
-      <c r="E139" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="F139" s="10">
-        <v>0</v>
-      </c>
-      <c r="G139" s="9" t="s">
-        <v>315</v>
       </c>
       <c r="H139" s="9" t="s">
         <v>31</v>
@@ -5656,25 +5644,25 @@
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A140" s="8" t="s">
+        <v>323</v>
+      </c>
+      <c r="B140" s="9" t="s">
         <v>324</v>
       </c>
-      <c r="B140" s="9" t="s">
-        <v>190</v>
-      </c>
       <c r="C140" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D140" s="9" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="E140" s="9" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="F140" s="10">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G140" s="9" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="H140" s="9" t="s">
         <v>31</v>
@@ -5688,19 +5676,19 @@
         <v>326</v>
       </c>
       <c r="C141" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D141" s="9" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="E141" s="9" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="F141" s="10">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="G141" s="9" t="s">
-        <v>315</v>
+        <v>327</v>
       </c>
       <c r="H141" s="9" t="s">
         <v>31</v>
@@ -5708,25 +5696,25 @@
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A142" s="8" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B142" s="9" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="C142" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D142" s="9" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="E142" s="9" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="F142" s="10">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G142" s="9" t="s">
-        <v>75</v>
+        <v>330</v>
       </c>
       <c r="H142" s="9" t="s">
         <v>31</v>
@@ -5734,25 +5722,25 @@
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A143" s="8" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="B143" s="9" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="C143" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D143" s="9" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="E143" s="9" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="F143" s="10">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G143" s="9" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="H143" s="9" t="s">
         <v>31</v>
@@ -5760,25 +5748,25 @@
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A144" s="8" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="B144" s="9" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="C144" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D144" s="9" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="E144" s="9" t="s">
         <v>25</v>
       </c>
       <c r="F144" s="10">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="G144" s="9" t="s">
-        <v>334</v>
+        <v>54</v>
       </c>
       <c r="H144" s="9" t="s">
         <v>31</v>
@@ -5786,25 +5774,25 @@
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A145" s="8" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B145" s="9" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C145" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D145" s="9" t="s">
-        <v>311</v>
+        <v>338</v>
       </c>
       <c r="E145" s="9" t="s">
-        <v>44</v>
+        <v>17</v>
       </c>
       <c r="F145" s="10">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G145" s="9" t="s">
-        <v>337</v>
+        <v>88</v>
       </c>
       <c r="H145" s="9" t="s">
         <v>31</v>
@@ -5812,25 +5800,25 @@
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A146" s="8" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B146" s="9" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="C146" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D146" s="9" t="s">
-        <v>311</v>
+        <v>341</v>
       </c>
       <c r="E146" s="9" t="s">
         <v>25</v>
       </c>
       <c r="F146" s="10">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="G146" s="9" t="s">
-        <v>54</v>
+        <v>88</v>
       </c>
       <c r="H146" s="9" t="s">
         <v>31</v>
@@ -5838,19 +5826,19 @@
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A147" s="8" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="B147" s="9" t="s">
+        <v>343</v>
+      </c>
+      <c r="C147" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="D147" s="9" t="s">
         <v>341</v>
       </c>
-      <c r="C147" s="9" t="s">
-        <v>289</v>
-      </c>
-      <c r="D147" s="9" t="s">
-        <v>342</v>
-      </c>
       <c r="E147" s="9" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="F147" s="10">
         <v>0</v>
@@ -5864,16 +5852,16 @@
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A148" s="8" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="B148" s="9" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="C148" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D148" s="9" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="E148" s="9" t="s">
         <v>25</v>
@@ -5893,16 +5881,16 @@
         <v>346</v>
       </c>
       <c r="B149" s="9" t="s">
-        <v>347</v>
+        <v>299</v>
       </c>
       <c r="C149" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D149" s="9" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="E149" s="9" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="F149" s="10">
         <v>0</v>
@@ -5916,16 +5904,16 @@
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A150" s="8" t="s">
+        <v>347</v>
+      </c>
+      <c r="B150" s="9" t="s">
         <v>348</v>
       </c>
-      <c r="B150" s="9" t="s">
-        <v>349</v>
-      </c>
       <c r="C150" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D150" s="9" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="E150" s="9" t="s">
         <v>25</v>
@@ -5942,103 +5930,103 @@
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A151" s="8" t="s">
+        <v>349</v>
+      </c>
+      <c r="B151" s="9" t="s">
         <v>350</v>
       </c>
-      <c r="B151" s="9" t="s">
-        <v>301</v>
-      </c>
       <c r="C151" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D151" s="9" t="s">
-        <v>345</v>
+        <v>351</v>
       </c>
       <c r="E151" s="9" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="F151" s="10">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G151" s="9" t="s">
-        <v>88</v>
+        <v>352</v>
       </c>
       <c r="H151" s="9" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A152" s="8" t="s">
-        <v>351</v>
-      </c>
-      <c r="B152" s="9" t="s">
-        <v>352</v>
-      </c>
-      <c r="C152" s="9" t="s">
-        <v>289</v>
-      </c>
-      <c r="D152" s="9" t="s">
-        <v>345</v>
-      </c>
-      <c r="E152" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="F152" s="10">
-        <v>0</v>
-      </c>
-      <c r="G152" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="H152" s="9" t="s">
-        <v>31</v>
+      <c r="A152" s="11" t="s">
+        <v>353</v>
+      </c>
+      <c r="B152" s="12" t="s">
+        <v>354</v>
+      </c>
+      <c r="C152" s="12" t="s">
+        <v>355</v>
+      </c>
+      <c r="D152" s="12" t="s">
+        <v>356</v>
+      </c>
+      <c r="E152" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="F152" s="13">
+        <v>0</v>
+      </c>
+      <c r="G152" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H152" s="12" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A153" s="8" t="s">
-        <v>353</v>
-      </c>
-      <c r="B153" s="9" t="s">
-        <v>354</v>
-      </c>
-      <c r="C153" s="9" t="s">
-        <v>289</v>
-      </c>
-      <c r="D153" s="9" t="s">
+      <c r="A153" s="11" t="s">
+        <v>357</v>
+      </c>
+      <c r="B153" s="12" t="s">
+        <v>358</v>
+      </c>
+      <c r="C153" s="12" t="s">
         <v>355</v>
       </c>
-      <c r="E153" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="F153" s="10">
-        <v>100</v>
-      </c>
-      <c r="G153" s="9" t="s">
+      <c r="D153" s="12" t="s">
         <v>356</v>
       </c>
-      <c r="H153" s="9" t="s">
-        <v>31</v>
+      <c r="E153" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="F153" s="13">
+        <v>0</v>
+      </c>
+      <c r="G153" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H153" s="12" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A154" s="11" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="B154" s="12" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="C154" s="12" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="D154" s="12" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="E154" s="12" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="F154" s="13">
         <v>0</v>
       </c>
       <c r="G154" s="12" t="s">
-        <v>20</v>
+        <v>111</v>
       </c>
       <c r="H154" s="12" t="s">
         <v>14</v>
@@ -6052,19 +6040,19 @@
         <v>362</v>
       </c>
       <c r="C155" s="12" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="D155" s="12" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="E155" s="12" t="s">
-        <v>81</v>
+        <v>17</v>
       </c>
       <c r="F155" s="13">
         <v>0</v>
       </c>
       <c r="G155" s="12" t="s">
-        <v>20</v>
+        <v>111</v>
       </c>
       <c r="H155" s="12" t="s">
         <v>14</v>
@@ -6075,13 +6063,13 @@
         <v>363</v>
       </c>
       <c r="B156" s="12" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="C156" s="12" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="D156" s="12" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="E156" s="12" t="s">
         <v>84</v>
@@ -6098,28 +6086,28 @@
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A157" s="11" t="s">
+        <v>364</v>
+      </c>
+      <c r="B157" s="12" t="s">
         <v>365</v>
       </c>
-      <c r="B157" s="12" t="s">
+      <c r="C157" s="12" t="s">
+        <v>355</v>
+      </c>
+      <c r="D157" s="12" t="s">
+        <v>356</v>
+      </c>
+      <c r="E157" s="12" t="s">
         <v>366</v>
       </c>
-      <c r="C157" s="12" t="s">
-        <v>359</v>
-      </c>
-      <c r="D157" s="12" t="s">
-        <v>360</v>
-      </c>
-      <c r="E157" s="12" t="s">
-        <v>17</v>
-      </c>
       <c r="F157" s="13">
         <v>0</v>
       </c>
       <c r="G157" s="12" t="s">
-        <v>111</v>
+        <v>75</v>
       </c>
       <c r="H157" s="12" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.3">
@@ -6127,22 +6115,22 @@
         <v>367</v>
       </c>
       <c r="B158" s="12" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="C158" s="12" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="D158" s="12" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="E158" s="12" t="s">
-        <v>84</v>
+        <v>17</v>
       </c>
       <c r="F158" s="13">
         <v>0</v>
       </c>
       <c r="G158" s="12" t="s">
-        <v>111</v>
+        <v>20</v>
       </c>
       <c r="H158" s="12" t="s">
         <v>14</v>
@@ -6156,22 +6144,22 @@
         <v>369</v>
       </c>
       <c r="C159" s="12" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="D159" s="12" t="s">
-        <v>360</v>
+        <v>370</v>
       </c>
       <c r="E159" s="12" t="s">
-        <v>370</v>
+        <v>84</v>
       </c>
       <c r="F159" s="13">
         <v>0</v>
       </c>
       <c r="G159" s="12" t="s">
-        <v>75</v>
+        <v>308</v>
       </c>
       <c r="H159" s="12" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.3">
@@ -6179,13 +6167,13 @@
         <v>371</v>
       </c>
       <c r="B160" s="12" t="s">
-        <v>362</v>
+        <v>372</v>
       </c>
       <c r="C160" s="12" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="D160" s="12" t="s">
-        <v>360</v>
+        <v>370</v>
       </c>
       <c r="E160" s="12" t="s">
         <v>17</v>
@@ -6202,16 +6190,16 @@
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A161" s="11" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="B161" s="12" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="C161" s="12" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="D161" s="12" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="E161" s="12" t="s">
         <v>84</v>
@@ -6220,7 +6208,7 @@
         <v>0</v>
       </c>
       <c r="G161" s="12" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="H161" s="12" t="s">
         <v>14</v>
@@ -6234,19 +6222,19 @@
         <v>376</v>
       </c>
       <c r="C162" s="12" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="D162" s="12" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="E162" s="12" t="s">
-        <v>17</v>
+        <v>81</v>
       </c>
       <c r="F162" s="13">
         <v>0</v>
       </c>
       <c r="G162" s="12" t="s">
-        <v>20</v>
+        <v>308</v>
       </c>
       <c r="H162" s="12" t="s">
         <v>14</v>
@@ -6260,10 +6248,10 @@
         <v>378</v>
       </c>
       <c r="C163" s="12" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="D163" s="12" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="E163" s="12" t="s">
         <v>84</v>
@@ -6272,7 +6260,7 @@
         <v>0</v>
       </c>
       <c r="G163" s="12" t="s">
-        <v>312</v>
+        <v>75</v>
       </c>
       <c r="H163" s="12" t="s">
         <v>14</v>
@@ -6286,19 +6274,19 @@
         <v>380</v>
       </c>
       <c r="C164" s="12" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="D164" s="12" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="E164" s="12" t="s">
-        <v>81</v>
+        <v>17</v>
       </c>
       <c r="F164" s="13">
-        <v>0</v>
+        <v>220</v>
       </c>
       <c r="G164" s="12" t="s">
-        <v>312</v>
+        <v>20</v>
       </c>
       <c r="H164" s="12" t="s">
         <v>14</v>
@@ -6312,10 +6300,10 @@
         <v>382</v>
       </c>
       <c r="C165" s="12" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="D165" s="12" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="E165" s="12" t="s">
         <v>84</v>
@@ -6324,7 +6312,7 @@
         <v>0</v>
       </c>
       <c r="G165" s="12" t="s">
-        <v>75</v>
+        <v>308</v>
       </c>
       <c r="H165" s="12" t="s">
         <v>14</v>
@@ -6338,22 +6326,22 @@
         <v>384</v>
       </c>
       <c r="C166" s="12" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="D166" s="12" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="E166" s="12" t="s">
         <v>17</v>
       </c>
       <c r="F166" s="13">
-        <v>220</v>
+        <v>0</v>
       </c>
       <c r="G166" s="12" t="s">
-        <v>20</v>
+        <v>111</v>
       </c>
       <c r="H166" s="12" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.3">
@@ -6364,19 +6352,19 @@
         <v>386</v>
       </c>
       <c r="C167" s="12" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="D167" s="12" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="E167" s="12" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F167" s="13">
         <v>0</v>
       </c>
       <c r="G167" s="12" t="s">
-        <v>312</v>
+        <v>387</v>
       </c>
       <c r="H167" s="12" t="s">
         <v>14</v>
@@ -6384,51 +6372,51 @@
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A168" s="11" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="B168" s="12" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="C168" s="12" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="D168" s="12" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="E168" s="12" t="s">
-        <v>17</v>
+        <v>84</v>
       </c>
       <c r="F168" s="13">
         <v>0</v>
       </c>
       <c r="G168" s="12" t="s">
-        <v>111</v>
+        <v>75</v>
       </c>
       <c r="H168" s="12" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A169" s="11" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B169" s="12" t="s">
-        <v>390</v>
+        <v>378</v>
       </c>
       <c r="C169" s="12" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="D169" s="12" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="E169" s="12" t="s">
-        <v>81</v>
+        <v>12</v>
       </c>
       <c r="F169" s="13">
         <v>0</v>
       </c>
       <c r="G169" s="12" t="s">
-        <v>391</v>
+        <v>20</v>
       </c>
       <c r="H169" s="12" t="s">
         <v>14</v>
@@ -6436,16 +6424,16 @@
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A170" s="11" t="s">
+        <v>391</v>
+      </c>
+      <c r="B170" s="12" t="s">
         <v>392</v>
       </c>
-      <c r="B170" s="12" t="s">
-        <v>393</v>
-      </c>
       <c r="C170" s="12" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="D170" s="12" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="E170" s="12" t="s">
         <v>84</v>
@@ -6454,7 +6442,7 @@
         <v>0</v>
       </c>
       <c r="G170" s="12" t="s">
-        <v>75</v>
+        <v>308</v>
       </c>
       <c r="H170" s="12" t="s">
         <v>14</v>
@@ -6462,25 +6450,25 @@
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A171" s="11" t="s">
+        <v>393</v>
+      </c>
+      <c r="B171" s="12" t="s">
         <v>394</v>
       </c>
-      <c r="B171" s="12" t="s">
-        <v>382</v>
-      </c>
       <c r="C171" s="12" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="D171" s="12" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="E171" s="12" t="s">
-        <v>12</v>
+        <v>84</v>
       </c>
       <c r="F171" s="13">
         <v>0</v>
       </c>
       <c r="G171" s="12" t="s">
-        <v>20</v>
+        <v>308</v>
       </c>
       <c r="H171" s="12" t="s">
         <v>14</v>
@@ -6494,10 +6482,10 @@
         <v>396</v>
       </c>
       <c r="C172" s="12" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="D172" s="12" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="E172" s="12" t="s">
         <v>84</v>
@@ -6506,7 +6494,7 @@
         <v>0</v>
       </c>
       <c r="G172" s="12" t="s">
-        <v>312</v>
+        <v>20</v>
       </c>
       <c r="H172" s="12" t="s">
         <v>14</v>
@@ -6520,10 +6508,10 @@
         <v>398</v>
       </c>
       <c r="C173" s="12" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="D173" s="12" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="E173" s="12" t="s">
         <v>84</v>
@@ -6532,7 +6520,7 @@
         <v>0</v>
       </c>
       <c r="G173" s="12" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="H173" s="12" t="s">
         <v>14</v>
@@ -6546,10 +6534,10 @@
         <v>400</v>
       </c>
       <c r="C174" s="12" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="D174" s="12" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="E174" s="12" t="s">
         <v>84</v>
@@ -6558,7 +6546,7 @@
         <v>0</v>
       </c>
       <c r="G174" s="12" t="s">
-        <v>20</v>
+        <v>308</v>
       </c>
       <c r="H174" s="12" t="s">
         <v>14</v>
@@ -6572,10 +6560,10 @@
         <v>402</v>
       </c>
       <c r="C175" s="12" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="D175" s="12" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="E175" s="12" t="s">
         <v>84</v>
@@ -6584,7 +6572,7 @@
         <v>0</v>
       </c>
       <c r="G175" s="12" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="H175" s="12" t="s">
         <v>14</v>
@@ -6598,10 +6586,10 @@
         <v>404</v>
       </c>
       <c r="C176" s="12" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="D176" s="12" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="E176" s="12" t="s">
         <v>84</v>
@@ -6610,7 +6598,7 @@
         <v>0</v>
       </c>
       <c r="G176" s="12" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="H176" s="12" t="s">
         <v>14</v>
@@ -6621,13 +6609,13 @@
         <v>405</v>
       </c>
       <c r="B177" s="12" t="s">
-        <v>406</v>
+        <v>147</v>
       </c>
       <c r="C177" s="12" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="D177" s="12" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="E177" s="12" t="s">
         <v>84</v>
@@ -6636,7 +6624,7 @@
         <v>0</v>
       </c>
       <c r="G177" s="12" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="H177" s="12" t="s">
         <v>14</v>
@@ -6644,25 +6632,25 @@
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A178" s="11" t="s">
+        <v>406</v>
+      </c>
+      <c r="B178" s="12" t="s">
         <v>407</v>
       </c>
-      <c r="B178" s="12" t="s">
-        <v>408</v>
-      </c>
       <c r="C178" s="12" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="D178" s="12" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="E178" s="12" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F178" s="13">
         <v>0</v>
       </c>
       <c r="G178" s="12" t="s">
-        <v>312</v>
+        <v>20</v>
       </c>
       <c r="H178" s="12" t="s">
         <v>14</v>
@@ -6670,25 +6658,25 @@
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A179" s="11" t="s">
+        <v>408</v>
+      </c>
+      <c r="B179" s="12" t="s">
         <v>409</v>
       </c>
-      <c r="B179" s="12" t="s">
-        <v>147</v>
-      </c>
       <c r="C179" s="12" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="D179" s="12" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="E179" s="12" t="s">
-        <v>84</v>
+        <v>12</v>
       </c>
       <c r="F179" s="13">
-        <v>0</v>
+        <v>220</v>
       </c>
       <c r="G179" s="12" t="s">
-        <v>312</v>
+        <v>20</v>
       </c>
       <c r="H179" s="12" t="s">
         <v>14</v>
@@ -6702,88 +6690,88 @@
         <v>411</v>
       </c>
       <c r="C180" s="12" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="D180" s="12" t="s">
-        <v>374</v>
+        <v>412</v>
       </c>
       <c r="E180" s="12" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="F180" s="13">
         <v>0</v>
       </c>
       <c r="G180" s="12" t="s">
-        <v>20</v>
+        <v>111</v>
       </c>
       <c r="H180" s="12" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A181" s="11" t="s">
-        <v>412</v>
-      </c>
-      <c r="B181" s="12" t="s">
+      <c r="A181" s="14" t="s">
         <v>413</v>
       </c>
-      <c r="C181" s="12" t="s">
-        <v>359</v>
-      </c>
-      <c r="D181" s="12" t="s">
-        <v>374</v>
-      </c>
-      <c r="E181" s="12" t="s">
+      <c r="B181" s="15" t="s">
+        <v>414</v>
+      </c>
+      <c r="C181" s="15" t="s">
+        <v>415</v>
+      </c>
+      <c r="D181" s="15" t="s">
+        <v>416</v>
+      </c>
+      <c r="E181" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="F181" s="13">
-        <v>220</v>
-      </c>
-      <c r="G181" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="H181" s="12" t="s">
-        <v>14</v>
+      <c r="F181" s="16">
+        <v>0</v>
+      </c>
+      <c r="G181" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="H181" s="15" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A182" s="11" t="s">
+      <c r="A182" s="14" t="s">
+        <v>417</v>
+      </c>
+      <c r="B182" s="15" t="s">
+        <v>418</v>
+      </c>
+      <c r="C182" s="15" t="s">
+        <v>415</v>
+      </c>
+      <c r="D182" s="15" t="s">
+        <v>416</v>
+      </c>
+      <c r="E182" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="F182" s="16">
+        <v>0</v>
+      </c>
+      <c r="G182" s="15" t="s">
+        <v>419</v>
+      </c>
+      <c r="H182" s="15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="183" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="A183" s="14" t="s">
+        <v>420</v>
+      </c>
+      <c r="B183" s="15" t="s">
         <v>414</v>
       </c>
-      <c r="B182" s="12" t="s">
+      <c r="C183" s="15" t="s">
         <v>415</v>
       </c>
-      <c r="C182" s="12" t="s">
-        <v>359</v>
-      </c>
-      <c r="D182" s="12" t="s">
+      <c r="D183" s="15" t="s">
         <v>416</v>
-      </c>
-      <c r="E182" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="F182" s="13">
-        <v>0</v>
-      </c>
-      <c r="G182" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="H182" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A183" s="14" t="s">
-        <v>417</v>
-      </c>
-      <c r="B183" s="15" t="s">
-        <v>418</v>
-      </c>
-      <c r="C183" s="15" t="s">
-        <v>419</v>
-      </c>
-      <c r="D183" s="15" t="s">
-        <v>420</v>
       </c>
       <c r="E183" s="15" t="s">
         <v>12</v>
@@ -6795,7 +6783,7 @@
         <v>13</v>
       </c>
       <c r="H183" s="15" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
     </row>
     <row r="184" spans="1:8" x14ac:dyDescent="0.3">
@@ -6806,10 +6794,10 @@
         <v>422</v>
       </c>
       <c r="C184" s="15" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="D184" s="15" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E184" s="15" t="s">
         <v>25</v>
@@ -6824,27 +6812,27 @@
         <v>31</v>
       </c>
     </row>
-    <row r="185" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A185" s="14" t="s">
         <v>424</v>
       </c>
       <c r="B185" s="15" t="s">
-        <v>418</v>
+        <v>147</v>
       </c>
       <c r="C185" s="15" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="D185" s="15" t="s">
-        <v>420</v>
+        <v>425</v>
       </c>
       <c r="E185" s="15" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="F185" s="16">
         <v>0</v>
       </c>
       <c r="G185" s="15" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="H185" s="15" t="s">
         <v>14</v>
@@ -6852,28 +6840,28 @@
     </row>
     <row r="186" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A186" s="14" t="s">
+        <v>426</v>
+      </c>
+      <c r="B186" s="15" t="s">
+        <v>427</v>
+      </c>
+      <c r="C186" s="15" t="s">
+        <v>415</v>
+      </c>
+      <c r="D186" s="15" t="s">
         <v>425</v>
       </c>
-      <c r="B186" s="15" t="s">
-        <v>426</v>
-      </c>
-      <c r="C186" s="15" t="s">
+      <c r="E186" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="F186" s="16">
+        <v>0</v>
+      </c>
+      <c r="G186" s="15" t="s">
         <v>419</v>
       </c>
-      <c r="D186" s="15" t="s">
-        <v>420</v>
-      </c>
-      <c r="E186" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="F186" s="16">
-        <v>0</v>
-      </c>
-      <c r="G186" s="15" t="s">
-        <v>427</v>
-      </c>
       <c r="H186" s="15" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
     </row>
     <row r="187" spans="1:8" x14ac:dyDescent="0.3">
@@ -6881,22 +6869,22 @@
         <v>428</v>
       </c>
       <c r="B187" s="15" t="s">
-        <v>147</v>
+        <v>429</v>
       </c>
       <c r="C187" s="15" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="D187" s="15" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="E187" s="15" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="F187" s="16">
         <v>0</v>
       </c>
       <c r="G187" s="15" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="H187" s="15" t="s">
         <v>14</v>
@@ -6907,25 +6895,25 @@
         <v>430</v>
       </c>
       <c r="B188" s="15" t="s">
+        <v>348</v>
+      </c>
+      <c r="C188" s="15" t="s">
+        <v>415</v>
+      </c>
+      <c r="D188" s="15" t="s">
         <v>431</v>
       </c>
-      <c r="C188" s="15" t="s">
-        <v>419</v>
-      </c>
-      <c r="D188" s="15" t="s">
-        <v>429</v>
-      </c>
       <c r="E188" s="15" t="s">
-        <v>81</v>
+        <v>25</v>
       </c>
       <c r="F188" s="16">
         <v>0</v>
       </c>
       <c r="G188" s="15" t="s">
-        <v>423</v>
+        <v>26</v>
       </c>
       <c r="H188" s="15" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
     </row>
     <row r="189" spans="1:8" x14ac:dyDescent="0.3">
@@ -6936,19 +6924,19 @@
         <v>433</v>
       </c>
       <c r="C189" s="15" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="D189" s="15" t="s">
-        <v>429</v>
+        <v>434</v>
       </c>
       <c r="E189" s="15" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="F189" s="16">
         <v>0</v>
       </c>
       <c r="G189" s="15" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="H189" s="15" t="s">
         <v>14</v>
@@ -6956,51 +6944,51 @@
     </row>
     <row r="190" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A190" s="14" t="s">
+        <v>435</v>
+      </c>
+      <c r="B190" s="15" t="s">
+        <v>436</v>
+      </c>
+      <c r="C190" s="15" t="s">
+        <v>415</v>
+      </c>
+      <c r="D190" s="15" t="s">
         <v>434</v>
       </c>
-      <c r="B190" s="15" t="s">
-        <v>352</v>
-      </c>
-      <c r="C190" s="15" t="s">
-        <v>419</v>
-      </c>
-      <c r="D190" s="15" t="s">
-        <v>435</v>
-      </c>
       <c r="E190" s="15" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="F190" s="16">
         <v>0</v>
       </c>
       <c r="G190" s="15" t="s">
-        <v>26</v>
+        <v>330</v>
       </c>
       <c r="H190" s="15" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
     </row>
     <row r="191" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A191" s="14" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="B191" s="15" t="s">
-        <v>437</v>
+        <v>42</v>
       </c>
       <c r="C191" s="15" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="D191" s="15" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="E191" s="15" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="F191" s="16">
         <v>0</v>
       </c>
       <c r="G191" s="15" t="s">
-        <v>26</v>
+        <v>330</v>
       </c>
       <c r="H191" s="15" t="s">
         <v>14</v>
@@ -7008,25 +6996,25 @@
     </row>
     <row r="192" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A192" s="14" t="s">
+        <v>438</v>
+      </c>
+      <c r="B192" s="15" t="s">
         <v>439</v>
       </c>
-      <c r="B192" s="15" t="s">
-        <v>440</v>
-      </c>
       <c r="C192" s="15" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="D192" s="15" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="E192" s="15" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="F192" s="16">
         <v>0</v>
       </c>
       <c r="G192" s="15" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="H192" s="15" t="s">
         <v>14</v>
@@ -7034,51 +7022,51 @@
     </row>
     <row r="193" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A193" s="14" t="s">
+        <v>440</v>
+      </c>
+      <c r="B193" s="15" t="s">
         <v>441</v>
       </c>
-      <c r="B193" s="15" t="s">
-        <v>42</v>
-      </c>
       <c r="C193" s="15" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="D193" s="15" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="E193" s="15" t="s">
-        <v>44</v>
+        <v>12</v>
       </c>
       <c r="F193" s="16">
         <v>0</v>
       </c>
       <c r="G193" s="15" t="s">
-        <v>334</v>
+        <v>442</v>
       </c>
       <c r="H193" s="15" t="s">
-        <v>14</v>
+        <v>443</v>
       </c>
     </row>
     <row r="194" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A194" s="14" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="B194" s="15" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="C194" s="15" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="D194" s="15" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="E194" s="15" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="F194" s="16">
         <v>0</v>
       </c>
       <c r="G194" s="15" t="s">
-        <v>334</v>
+        <v>26</v>
       </c>
       <c r="H194" s="15" t="s">
         <v>14</v>
@@ -7086,28 +7074,28 @@
     </row>
     <row r="195" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A195" s="14" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="B195" s="15" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="C195" s="15" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="D195" s="15" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="E195" s="15" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="F195" s="16">
         <v>0</v>
       </c>
       <c r="G195" s="15" t="s">
-        <v>446</v>
+        <v>26</v>
       </c>
       <c r="H195" s="15" t="s">
-        <v>447</v>
+        <v>14</v>
       </c>
     </row>
     <row r="196" spans="1:8" x14ac:dyDescent="0.3">
@@ -7118,19 +7106,19 @@
         <v>449</v>
       </c>
       <c r="C196" s="15" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="D196" s="15" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="E196" s="15" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="F196" s="16">
         <v>0</v>
       </c>
       <c r="G196" s="15" t="s">
-        <v>26</v>
+        <v>330</v>
       </c>
       <c r="H196" s="15" t="s">
         <v>14</v>
@@ -7144,19 +7132,19 @@
         <v>451</v>
       </c>
       <c r="C197" s="15" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="D197" s="15" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="E197" s="15" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="F197" s="16">
         <v>0</v>
       </c>
       <c r="G197" s="15" t="s">
-        <v>26</v>
+        <v>330</v>
       </c>
       <c r="H197" s="15" t="s">
         <v>14</v>
@@ -7170,19 +7158,19 @@
         <v>453</v>
       </c>
       <c r="C198" s="15" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="D198" s="15" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="E198" s="15" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="F198" s="16">
         <v>0</v>
       </c>
       <c r="G198" s="15" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="H198" s="15" t="s">
         <v>14</v>
@@ -7196,19 +7184,19 @@
         <v>455</v>
       </c>
       <c r="C199" s="15" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="D199" s="15" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="E199" s="15" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="F199" s="16">
         <v>0</v>
       </c>
       <c r="G199" s="15" t="s">
-        <v>334</v>
+        <v>26</v>
       </c>
       <c r="H199" s="15" t="s">
         <v>14</v>
@@ -7222,36 +7210,36 @@
         <v>457</v>
       </c>
       <c r="C200" s="15" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="D200" s="15" t="s">
-        <v>438</v>
+        <v>458</v>
       </c>
       <c r="E200" s="15" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="F200" s="16">
         <v>0</v>
       </c>
       <c r="G200" s="15" t="s">
-        <v>334</v>
+        <v>26</v>
       </c>
       <c r="H200" s="15" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
     </row>
     <row r="201" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A201" s="14" t="s">
+        <v>459</v>
+      </c>
+      <c r="B201" s="15" t="s">
+        <v>460</v>
+      </c>
+      <c r="C201" s="15" t="s">
+        <v>415</v>
+      </c>
+      <c r="D201" s="15" t="s">
         <v>458</v>
-      </c>
-      <c r="B201" s="15" t="s">
-        <v>459</v>
-      </c>
-      <c r="C201" s="15" t="s">
-        <v>419</v>
-      </c>
-      <c r="D201" s="15" t="s">
-        <v>438</v>
       </c>
       <c r="E201" s="15" t="s">
         <v>25</v>
@@ -7260,33 +7248,33 @@
         <v>0</v>
       </c>
       <c r="G201" s="15" t="s">
-        <v>26</v>
+        <v>461</v>
       </c>
       <c r="H201" s="15" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
     </row>
     <row r="202" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A202" s="14" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="B202" s="15" t="s">
-        <v>461</v>
+        <v>83</v>
       </c>
       <c r="C202" s="15" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="D202" s="15" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="E202" s="15" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="F202" s="16">
         <v>0</v>
       </c>
       <c r="G202" s="15" t="s">
-        <v>26</v>
+        <v>311</v>
       </c>
       <c r="H202" s="15" t="s">
         <v>31</v>
@@ -7297,22 +7285,22 @@
         <v>463</v>
       </c>
       <c r="B203" s="15" t="s">
-        <v>464</v>
+        <v>90</v>
       </c>
       <c r="C203" s="15" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="D203" s="15" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="E203" s="15" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="F203" s="16">
         <v>0</v>
       </c>
       <c r="G203" s="15" t="s">
-        <v>465</v>
+        <v>26</v>
       </c>
       <c r="H203" s="15" t="s">
         <v>31</v>
@@ -7320,25 +7308,25 @@
     </row>
     <row r="204" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A204" s="14" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="B204" s="15" t="s">
-        <v>83</v>
+        <v>465</v>
       </c>
       <c r="C204" s="15" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="D204" s="15" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="E204" s="15" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="F204" s="16">
         <v>0</v>
       </c>
       <c r="G204" s="15" t="s">
-        <v>315</v>
+        <v>69</v>
       </c>
       <c r="H204" s="15" t="s">
         <v>31</v>
@@ -7346,16 +7334,16 @@
     </row>
     <row r="205" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A205" s="14" t="s">
+        <v>466</v>
+      </c>
+      <c r="B205" s="15" t="s">
+        <v>429</v>
+      </c>
+      <c r="C205" s="15" t="s">
+        <v>415</v>
+      </c>
+      <c r="D205" s="15" t="s">
         <v>467</v>
-      </c>
-      <c r="B205" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="C205" s="15" t="s">
-        <v>419</v>
-      </c>
-      <c r="D205" s="15" t="s">
-        <v>462</v>
       </c>
       <c r="E205" s="15" t="s">
         <v>12</v>
@@ -7364,10 +7352,10 @@
         <v>0</v>
       </c>
       <c r="G205" s="15" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="H205" s="15" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
     </row>
     <row r="206" spans="1:8" x14ac:dyDescent="0.3">
@@ -7378,10 +7366,10 @@
         <v>469</v>
       </c>
       <c r="C206" s="15" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="D206" s="15" t="s">
-        <v>462</v>
+        <v>470</v>
       </c>
       <c r="E206" s="15" t="s">
         <v>12</v>
@@ -7390,7 +7378,7 @@
         <v>0</v>
       </c>
       <c r="G206" s="15" t="s">
-        <v>69</v>
+        <v>419</v>
       </c>
       <c r="H206" s="15" t="s">
         <v>31</v>
@@ -7398,28 +7386,28 @@
     </row>
     <row r="207" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A207" s="14" t="s">
+        <v>471</v>
+      </c>
+      <c r="B207" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="C207" s="15" t="s">
+        <v>415</v>
+      </c>
+      <c r="D207" s="15" t="s">
         <v>470</v>
       </c>
-      <c r="B207" s="15" t="s">
-        <v>433</v>
-      </c>
-      <c r="C207" s="15" t="s">
-        <v>419</v>
-      </c>
-      <c r="D207" s="15" t="s">
-        <v>471</v>
-      </c>
       <c r="E207" s="15" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="F207" s="16">
         <v>0</v>
       </c>
       <c r="G207" s="15" t="s">
-        <v>20</v>
+        <v>88</v>
       </c>
       <c r="H207" s="15" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
     </row>
     <row r="208" spans="1:8" x14ac:dyDescent="0.3">
@@ -7427,22 +7415,22 @@
         <v>472</v>
       </c>
       <c r="B208" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="C208" s="15" t="s">
+        <v>415</v>
+      </c>
+      <c r="D208" s="15" t="s">
+        <v>470</v>
+      </c>
+      <c r="E208" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F208" s="16">
+        <v>0</v>
+      </c>
+      <c r="G208" s="15" t="s">
         <v>473</v>
-      </c>
-      <c r="C208" s="15" t="s">
-        <v>419</v>
-      </c>
-      <c r="D208" s="15" t="s">
-        <v>474</v>
-      </c>
-      <c r="E208" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="F208" s="16">
-        <v>0</v>
-      </c>
-      <c r="G208" s="15" t="s">
-        <v>423</v>
       </c>
       <c r="H208" s="15" t="s">
         <v>31</v>
@@ -7450,16 +7438,16 @@
     </row>
     <row r="209" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A209" s="14" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B209" s="15" t="s">
         <v>147</v>
       </c>
       <c r="C209" s="15" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="D209" s="15" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="E209" s="15" t="s">
         <v>17</v>
@@ -7468,92 +7456,40 @@
         <v>0</v>
       </c>
       <c r="G209" s="15" t="s">
-        <v>88</v>
+        <v>69</v>
       </c>
       <c r="H209" s="15" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
     </row>
     <row r="210" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A210" s="14" t="s">
+        <v>475</v>
+      </c>
+      <c r="B210" s="15" t="s">
         <v>476</v>
       </c>
-      <c r="B210" s="15" t="s">
-        <v>147</v>
-      </c>
       <c r="C210" s="15" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="D210" s="15" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="E210" s="15" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="F210" s="16">
         <v>0</v>
       </c>
       <c r="G210" s="15" t="s">
-        <v>477</v>
+        <v>69</v>
       </c>
       <c r="H210" s="15" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="211" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A211" s="14" t="s">
-        <v>478</v>
-      </c>
-      <c r="B211" s="15" t="s">
-        <v>147</v>
-      </c>
-      <c r="C211" s="15" t="s">
-        <v>419</v>
-      </c>
-      <c r="D211" s="15" t="s">
-        <v>474</v>
-      </c>
-      <c r="E211" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="F211" s="16">
-        <v>0</v>
-      </c>
-      <c r="G211" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="H211" s="15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="212" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A212" s="14" t="s">
-        <v>479</v>
-      </c>
-      <c r="B212" s="15" t="s">
-        <v>480</v>
-      </c>
-      <c r="C212" s="15" t="s">
-        <v>419</v>
-      </c>
-      <c r="D212" s="15" t="s">
-        <v>474</v>
-      </c>
-      <c r="E212" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="F212" s="16">
-        <v>0</v>
-      </c>
-      <c r="G212" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="H212" s="15" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H212" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:H210" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -7573,7 +7509,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="37" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="B1" s="38"/>
       <c r="C1" s="38"/>
@@ -7581,7 +7517,7 @@
     </row>
     <row r="3" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="B3" s="18">
         <v>218</v>
@@ -7592,10 +7528,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -7611,7 +7547,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="23" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B7" s="24">
         <v>34</v>
@@ -7622,7 +7558,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="26" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="B8" s="27">
         <v>31</v>
@@ -7633,7 +7569,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="29" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="B9" s="30">
         <v>29</v>
@@ -7655,18 +7591,18 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="35" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="B11" s="19">
         <v>218</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="36" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactor specific interest to inject selected POIs into itinerary by ID
</commit_message>
<xml_diff>
--- a/Cairo_Giza_POI_Database_v3.xlsx
+++ b/Cairo_Giza_POI_Database_v3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abraam Refaat\Downloads\travel-recommendation-api---main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9BC6FC9-095E-429A-8682-BC988D6AA562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E53BBC7-137F-4DAE-98B7-47F4FB0ED3B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2013,8 +2013,8 @@
   <dimension ref="A1:H210"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A197" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A108" sqref="A108:XFD108"/>
+      <pane ySplit="1" topLeftCell="A146" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D158" sqref="D158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Update POI database: replace NaNs with zeros
</commit_message>
<xml_diff>
--- a/Cairo_Giza_POI_Database_v3.xlsx
+++ b/Cairo_Giza_POI_Database_v3.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abd El Rahman\Documents\GitHub\Nile-Quest---Graduation-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abraam Refaat\Downloads\travel-recommendation-api---main\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{882B596E-7EE3-48CB-AC75-2CED58A3BD4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cairo &amp; Giza POIs" sheetId="1" r:id="rId1"/>
@@ -18,7 +19,20 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Cairo &amp; Giza POIs'!$A$1:$H$210</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1861,7 +1875,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0\%"/>
   </numFmts>
@@ -2361,12 +2375,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I260"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F79" sqref="F78:F79"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G261" sqref="G261"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8699,7 +8713,9 @@
       <c r="F211" s="4" t="s">
         <v>471</v>
       </c>
-      <c r="G211" s="5"/>
+      <c r="G211" s="5">
+        <v>0</v>
+      </c>
       <c r="H211" s="4" t="s">
         <v>472</v>
       </c>
@@ -8727,7 +8743,9 @@
       <c r="F212" s="4" t="s">
         <v>475</v>
       </c>
-      <c r="G212" s="5"/>
+      <c r="G212" s="5">
+        <v>0</v>
+      </c>
       <c r="H212" s="4" t="s">
         <v>448</v>
       </c>
@@ -8755,7 +8773,9 @@
       <c r="F213" s="4" t="s">
         <v>351</v>
       </c>
-      <c r="G213" s="5"/>
+      <c r="G213" s="5">
+        <v>0</v>
+      </c>
       <c r="H213" s="4" t="s">
         <v>316</v>
       </c>
@@ -8783,7 +8803,9 @@
       <c r="F214" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="G214" s="5"/>
+      <c r="G214" s="5">
+        <v>0</v>
+      </c>
       <c r="H214" s="4" t="s">
         <v>481</v>
       </c>
@@ -8811,7 +8833,9 @@
       <c r="F215" s="4" t="s">
         <v>485</v>
       </c>
-      <c r="G215" s="5"/>
+      <c r="G215" s="5">
+        <v>0</v>
+      </c>
       <c r="H215" s="4" t="s">
         <v>486</v>
       </c>
@@ -8839,7 +8863,9 @@
       <c r="F216" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G216" s="5"/>
+      <c r="G216" s="5">
+        <v>0</v>
+      </c>
       <c r="H216" s="4" t="s">
         <v>490</v>
       </c>
@@ -8867,7 +8893,9 @@
       <c r="F217" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G217" s="5"/>
+      <c r="G217" s="5">
+        <v>0</v>
+      </c>
       <c r="H217" s="4" t="s">
         <v>494</v>
       </c>
@@ -8895,7 +8923,9 @@
       <c r="F218" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G218" s="5"/>
+      <c r="G218" s="5">
+        <v>0</v>
+      </c>
       <c r="H218" s="4" t="s">
         <v>481</v>
       </c>
@@ -8923,7 +8953,9 @@
       <c r="F219" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G219" s="5"/>
+      <c r="G219" s="5">
+        <v>0</v>
+      </c>
       <c r="H219" s="4" t="s">
         <v>499</v>
       </c>
@@ -8951,7 +8983,9 @@
       <c r="F220" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G220" s="5"/>
+      <c r="G220" s="5">
+        <v>0</v>
+      </c>
       <c r="H220" s="4" t="s">
         <v>502</v>
       </c>
@@ -8979,7 +9013,9 @@
       <c r="F221" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G221" s="5"/>
+      <c r="G221" s="5">
+        <v>0</v>
+      </c>
       <c r="H221" s="4" t="s">
         <v>502</v>
       </c>
@@ -9007,7 +9043,9 @@
       <c r="F222" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G222" s="5"/>
+      <c r="G222" s="5">
+        <v>0</v>
+      </c>
       <c r="H222" s="4" t="s">
         <v>509</v>
       </c>
@@ -9035,7 +9073,9 @@
       <c r="F223" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G223" s="5"/>
+      <c r="G223" s="5">
+        <v>0</v>
+      </c>
       <c r="H223" s="4" t="s">
         <v>513</v>
       </c>
@@ -9063,7 +9103,9 @@
       <c r="F224" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G224" s="5"/>
+      <c r="G224" s="5">
+        <v>0</v>
+      </c>
       <c r="H224" s="4" t="s">
         <v>463</v>
       </c>
@@ -9091,7 +9133,9 @@
       <c r="F225" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G225" s="5"/>
+      <c r="G225" s="5">
+        <v>0</v>
+      </c>
       <c r="H225" s="4" t="s">
         <v>502</v>
       </c>
@@ -9119,7 +9163,9 @@
       <c r="F226" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G226" s="5"/>
+      <c r="G226" s="5">
+        <v>0</v>
+      </c>
       <c r="H226" s="4" t="s">
         <v>521</v>
       </c>
@@ -9147,7 +9193,9 @@
       <c r="F227" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G227" s="5"/>
+      <c r="G227" s="5">
+        <v>0</v>
+      </c>
       <c r="H227" s="4" t="s">
         <v>481</v>
       </c>
@@ -9175,7 +9223,9 @@
       <c r="F228" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="G228" s="5"/>
+      <c r="G228" s="5">
+        <v>0</v>
+      </c>
       <c r="H228" s="4" t="s">
         <v>499</v>
       </c>
@@ -9203,7 +9253,9 @@
       <c r="F229" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G229" s="5"/>
+      <c r="G229" s="5">
+        <v>0</v>
+      </c>
       <c r="H229" s="4" t="s">
         <v>499</v>
       </c>
@@ -9231,7 +9283,9 @@
       <c r="F230" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G230" s="5"/>
+      <c r="G230" s="5">
+        <v>0</v>
+      </c>
       <c r="H230" s="4" t="s">
         <v>486</v>
       </c>
@@ -9259,7 +9313,9 @@
       <c r="F231" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G231" s="5"/>
+      <c r="G231" s="5">
+        <v>0</v>
+      </c>
       <c r="H231" s="4" t="s">
         <v>502</v>
       </c>
@@ -9287,7 +9343,9 @@
       <c r="F232" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G232" s="5"/>
+      <c r="G232" s="5">
+        <v>0</v>
+      </c>
       <c r="H232" s="4" t="s">
         <v>499</v>
       </c>
@@ -9315,7 +9373,9 @@
       <c r="F233" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G233" s="5"/>
+      <c r="G233" s="5">
+        <v>0</v>
+      </c>
       <c r="H233" s="4" t="s">
         <v>481</v>
       </c>
@@ -9343,7 +9403,9 @@
       <c r="F234" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="G234" s="5"/>
+      <c r="G234" s="5">
+        <v>0</v>
+      </c>
       <c r="H234" s="4" t="s">
         <v>502</v>
       </c>
@@ -9371,7 +9433,9 @@
       <c r="F235" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="G235" s="5"/>
+      <c r="G235" s="5">
+        <v>0</v>
+      </c>
       <c r="H235" s="4" t="s">
         <v>502</v>
       </c>
@@ -9399,7 +9463,9 @@
       <c r="F236" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G236" s="5"/>
+      <c r="G236" s="5">
+        <v>0</v>
+      </c>
       <c r="H236" s="4" t="s">
         <v>521</v>
       </c>
@@ -9427,7 +9493,9 @@
       <c r="F237" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G237" s="5"/>
+      <c r="G237" s="5">
+        <v>0</v>
+      </c>
       <c r="H237" s="4" t="s">
         <v>521</v>
       </c>
@@ -9455,7 +9523,9 @@
       <c r="F238" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G238" s="5"/>
+      <c r="G238" s="5">
+        <v>0</v>
+      </c>
       <c r="H238" s="4" t="s">
         <v>463</v>
       </c>
@@ -9483,7 +9553,9 @@
       <c r="F239" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G239" s="5"/>
+      <c r="G239" s="5">
+        <v>0</v>
+      </c>
       <c r="H239" s="4" t="s">
         <v>293</v>
       </c>
@@ -9511,7 +9583,9 @@
       <c r="F240" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G240" s="5"/>
+      <c r="G240" s="5">
+        <v>0</v>
+      </c>
       <c r="H240" s="4" t="s">
         <v>293</v>
       </c>
@@ -9539,7 +9613,9 @@
       <c r="F241" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G241" s="5"/>
+      <c r="G241" s="5">
+        <v>0</v>
+      </c>
       <c r="H241" s="4" t="s">
         <v>502</v>
       </c>
@@ -9567,7 +9643,9 @@
       <c r="F242" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="G242" s="5"/>
+      <c r="G242" s="5">
+        <v>0</v>
+      </c>
       <c r="H242" s="4" t="s">
         <v>502</v>
       </c>
@@ -9595,7 +9673,9 @@
       <c r="F243" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="G243" s="5"/>
+      <c r="G243" s="5">
+        <v>0</v>
+      </c>
       <c r="H243" s="4" t="s">
         <v>481</v>
       </c>
@@ -9623,7 +9703,9 @@
       <c r="F244" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G244" s="5"/>
+      <c r="G244" s="5">
+        <v>0</v>
+      </c>
       <c r="H244" s="4" t="s">
         <v>502</v>
       </c>
@@ -9651,7 +9733,9 @@
       <c r="F245" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G245" s="5"/>
+      <c r="G245" s="5">
+        <v>0</v>
+      </c>
       <c r="H245" s="4" t="s">
         <v>481</v>
       </c>
@@ -9679,7 +9763,9 @@
       <c r="F246" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G246" s="5"/>
+      <c r="G246" s="5">
+        <v>0</v>
+      </c>
       <c r="H246" s="4" t="s">
         <v>481</v>
       </c>
@@ -9707,7 +9793,9 @@
       <c r="F247" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G247" s="5"/>
+      <c r="G247" s="5">
+        <v>0</v>
+      </c>
       <c r="H247" s="4" t="s">
         <v>481</v>
       </c>
@@ -9735,7 +9823,9 @@
       <c r="F248" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G248" s="5"/>
+      <c r="G248" s="5">
+        <v>0</v>
+      </c>
       <c r="H248" s="4" t="s">
         <v>521</v>
       </c>
@@ -9763,7 +9853,9 @@
       <c r="F249" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G249" s="5"/>
+      <c r="G249" s="5">
+        <v>0</v>
+      </c>
       <c r="H249" s="4" t="s">
         <v>293</v>
       </c>
@@ -9791,7 +9883,9 @@
       <c r="F250" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="G250" s="5"/>
+      <c r="G250" s="5">
+        <v>0</v>
+      </c>
       <c r="H250" s="4" t="s">
         <v>481</v>
       </c>
@@ -9819,7 +9913,9 @@
       <c r="F251" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G251" s="5"/>
+      <c r="G251" s="5">
+        <v>0</v>
+      </c>
       <c r="H251" s="4" t="s">
         <v>486</v>
       </c>
@@ -9847,7 +9943,9 @@
       <c r="F252" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G252" s="5"/>
+      <c r="G252" s="5">
+        <v>0</v>
+      </c>
       <c r="H252" s="4" t="s">
         <v>502</v>
       </c>
@@ -9875,7 +9973,9 @@
       <c r="F253" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G253" s="5"/>
+      <c r="G253" s="5">
+        <v>0</v>
+      </c>
       <c r="H253" s="4" t="s">
         <v>481</v>
       </c>
@@ -9903,7 +10003,9 @@
       <c r="F254" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G254" s="5"/>
+      <c r="G254" s="5">
+        <v>0</v>
+      </c>
       <c r="H254" s="4" t="s">
         <v>588</v>
       </c>
@@ -9931,7 +10033,9 @@
       <c r="F255" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G255" s="5"/>
+      <c r="G255" s="5">
+        <v>0</v>
+      </c>
       <c r="H255" s="4" t="s">
         <v>591</v>
       </c>
@@ -9959,7 +10063,9 @@
       <c r="F256" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G256" s="5"/>
+      <c r="G256" s="5">
+        <v>0</v>
+      </c>
       <c r="H256" s="4" t="s">
         <v>481</v>
       </c>
@@ -9987,7 +10093,9 @@
       <c r="F257" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G257" s="5"/>
+      <c r="G257" s="5">
+        <v>0</v>
+      </c>
       <c r="H257" s="4" t="s">
         <v>521</v>
       </c>
@@ -10015,7 +10123,9 @@
       <c r="F258" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G258" s="5"/>
+      <c r="G258" s="5">
+        <v>0</v>
+      </c>
       <c r="H258" s="4" t="s">
         <v>490</v>
       </c>
@@ -10043,7 +10153,9 @@
       <c r="F259" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G259" s="5"/>
+      <c r="G259" s="5">
+        <v>0</v>
+      </c>
       <c r="H259" s="4" t="s">
         <v>481</v>
       </c>
@@ -10071,7 +10183,9 @@
       <c r="F260" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="G260" s="5"/>
+      <c r="G260" s="5">
+        <v>0</v>
+      </c>
       <c r="H260" s="4" t="s">
         <v>316</v>
       </c>
@@ -10080,14 +10194,14 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H210"/>
+  <autoFilter ref="A1:H210" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>

</xml_diff>

<commit_message>
Integrate Qdrant vector search and update dependencies
</commit_message>
<xml_diff>
--- a/Cairo_Giza_POI_Database_v3.xlsx
+++ b/Cairo_Giza_POI_Database_v3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abraam Refaat\Downloads\travel-recommendation-api---main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{882B596E-7EE3-48CB-AC75-2CED58A3BD4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18A295EE-22C4-4AFF-B276-AC5CD6DC6F47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1835" uniqueCount="611">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1821" uniqueCount="606">
   <si>
     <t>ID</t>
   </si>
@@ -1788,12 +1788,6 @@
     <t>International, Seafood</t>
   </si>
   <si>
-    <t>Fish Market</t>
-  </si>
-  <si>
-    <t>Seafood, Egyptian</t>
-  </si>
-  <si>
     <t>Isola</t>
   </si>
   <si>
@@ -1804,15 +1798,6 @@
   </si>
   <si>
     <t>11:00 - 23:00</t>
-  </si>
-  <si>
-    <t>Paul</t>
-  </si>
-  <si>
-    <t>French, Bakery, Cafe</t>
-  </si>
-  <si>
-    <t>08:00 - 23:00</t>
   </si>
   <si>
     <t>La Fandi</t>
@@ -2376,11 +2361,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I260"/>
+  <dimension ref="A1:I258"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G261" sqref="G261"/>
+      <pane ySplit="1" topLeftCell="A211" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A236" sqref="A236:XFD236"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8185,7 +8170,7 @@
     </row>
     <row r="194" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A194" s="2">
-        <f t="shared" ref="A194:A260" si="3">ROW()-1</f>
+        <f t="shared" ref="A194:A258" si="3">ROW()-1</f>
         <v>193</v>
       </c>
       <c r="B194" s="15" t="s">
@@ -9923,7 +9908,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="252" spans="1:9" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A252" s="2">
         <f t="shared" si="3"/>
         <v>251</v>
@@ -9932,13 +9917,13 @@
         <v>583</v>
       </c>
       <c r="C252" s="4" t="s">
-        <v>66</v>
+        <v>584</v>
       </c>
       <c r="D252" s="4" t="s">
         <v>469</v>
       </c>
       <c r="E252" s="4" t="s">
-        <v>584</v>
+        <v>562</v>
       </c>
       <c r="F252" s="4" t="s">
         <v>13</v>
@@ -9947,10 +9932,10 @@
         <v>0</v>
       </c>
       <c r="H252" s="4" t="s">
-        <v>502</v>
+        <v>481</v>
       </c>
       <c r="I252" s="4" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="253" spans="1:9" x14ac:dyDescent="0.3">
@@ -9962,22 +9947,22 @@
         <v>585</v>
       </c>
       <c r="C253" s="4" t="s">
-        <v>586</v>
+        <v>66</v>
       </c>
       <c r="D253" s="4" t="s">
         <v>469</v>
       </c>
       <c r="E253" s="4" t="s">
-        <v>562</v>
+        <v>512</v>
       </c>
       <c r="F253" s="4" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="G253" s="5">
         <v>0</v>
       </c>
       <c r="H253" s="4" t="s">
-        <v>481</v>
+        <v>586</v>
       </c>
       <c r="I253" s="4" t="s">
         <v>15</v>
@@ -9992,13 +9977,13 @@
         <v>587</v>
       </c>
       <c r="C254" s="4" t="s">
-        <v>66</v>
+        <v>588</v>
       </c>
       <c r="D254" s="4" t="s">
         <v>469</v>
       </c>
       <c r="E254" s="4" t="s">
-        <v>512</v>
+        <v>493</v>
       </c>
       <c r="F254" s="4" t="s">
         <v>18</v>
@@ -10007,7 +9992,7 @@
         <v>0</v>
       </c>
       <c r="H254" s="4" t="s">
-        <v>588</v>
+        <v>481</v>
       </c>
       <c r="I254" s="4" t="s">
         <v>15</v>
@@ -10028,16 +10013,16 @@
         <v>469</v>
       </c>
       <c r="E255" s="4" t="s">
-        <v>590</v>
+        <v>533</v>
       </c>
       <c r="F255" s="4" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G255" s="5">
         <v>0</v>
       </c>
       <c r="H255" s="4" t="s">
-        <v>591</v>
+        <v>521</v>
       </c>
       <c r="I255" s="4" t="s">
         <v>15</v>
@@ -10049,25 +10034,25 @@
         <v>255</v>
       </c>
       <c r="B256" s="3" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="C256" s="4" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="D256" s="4" t="s">
         <v>469</v>
       </c>
       <c r="E256" s="4" t="s">
-        <v>493</v>
+        <v>592</v>
       </c>
       <c r="F256" s="4" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G256" s="5">
         <v>0</v>
       </c>
       <c r="H256" s="4" t="s">
-        <v>481</v>
+        <v>490</v>
       </c>
       <c r="I256" s="4" t="s">
         <v>15</v>
@@ -10079,25 +10064,25 @@
         <v>256</v>
       </c>
       <c r="B257" s="3" t="s">
+        <v>593</v>
+      </c>
+      <c r="C257" s="4" t="s">
         <v>594</v>
-      </c>
-      <c r="C257" s="4" t="s">
-        <v>66</v>
       </c>
       <c r="D257" s="4" t="s">
         <v>469</v>
       </c>
       <c r="E257" s="4" t="s">
-        <v>533</v>
+        <v>595</v>
       </c>
       <c r="F257" s="4" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="G257" s="5">
         <v>0</v>
       </c>
       <c r="H257" s="4" t="s">
-        <v>521</v>
+        <v>481</v>
       </c>
       <c r="I257" s="4" t="s">
         <v>15</v>
@@ -10109,87 +10094,27 @@
         <v>257</v>
       </c>
       <c r="B258" s="3" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="C258" s="4" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="D258" s="4" t="s">
         <v>469</v>
       </c>
       <c r="E258" s="4" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="F258" s="4" t="s">
-        <v>13</v>
+        <v>84</v>
       </c>
       <c r="G258" s="5">
         <v>0</v>
       </c>
       <c r="H258" s="4" t="s">
-        <v>490</v>
+        <v>316</v>
       </c>
       <c r="I258" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="259" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A259" s="2">
-        <f t="shared" si="3"/>
-        <v>258</v>
-      </c>
-      <c r="B259" s="3" t="s">
-        <v>598</v>
-      </c>
-      <c r="C259" s="4" t="s">
-        <v>599</v>
-      </c>
-      <c r="D259" s="4" t="s">
-        <v>469</v>
-      </c>
-      <c r="E259" s="4" t="s">
-        <v>600</v>
-      </c>
-      <c r="F259" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G259" s="5">
-        <v>0</v>
-      </c>
-      <c r="H259" s="4" t="s">
-        <v>481</v>
-      </c>
-      <c r="I259" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="260" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A260" s="2">
-        <f t="shared" si="3"/>
-        <v>259</v>
-      </c>
-      <c r="B260" s="3" t="s">
-        <v>601</v>
-      </c>
-      <c r="C260" s="4" t="s">
-        <v>602</v>
-      </c>
-      <c r="D260" s="4" t="s">
-        <v>469</v>
-      </c>
-      <c r="E260" s="4" t="s">
-        <v>603</v>
-      </c>
-      <c r="F260" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="G260" s="5">
-        <v>0</v>
-      </c>
-      <c r="H260" s="4" t="s">
-        <v>316</v>
-      </c>
-      <c r="I260" s="4" t="s">
         <v>15</v>
       </c>
     </row>
@@ -10215,7 +10140,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="38" t="s">
-        <v>604</v>
+        <v>599</v>
       </c>
       <c r="B1" s="39"/>
       <c r="C1" s="39"/>
@@ -10223,7 +10148,7 @@
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
-        <v>605</v>
+        <v>600</v>
       </c>
       <c r="B3" s="19">
         <v>259</v>
@@ -10234,10 +10159,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>606</v>
+        <v>601</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>607</v>
+        <v>602</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -10297,18 +10222,18 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="36" t="s">
-        <v>608</v>
+        <v>603</v>
       </c>
       <c r="B11" s="20">
         <v>218</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>609</v>
+        <v>604</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="37" t="s">
-        <v>610</v>
+        <v>605</v>
       </c>
     </row>
   </sheetData>

</xml_diff>